<commit_message>
added comet.params and added to README
</commit_message>
<xml_diff>
--- a/analysis_stats.xlsx
+++ b/analysis_stats.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\PXD014414\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pwilmart/Box Sync/Github_misc/analysis_example_repos/Metaplastic-BC_PXD014414/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5509552-9CFC-47EA-ABA8-B2B8441DDCFA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E168AE6-4DD2-EF4B-A639-584FA4FAA42D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15945" xr2:uid="{776DF520-25ED-4C4D-AE26-620CDD69525C}"/>
+    <workbookView xWindow="54300" yWindow="1680" windowWidth="29000" windowHeight="15940" xr2:uid="{776DF520-25ED-4C4D-AE26-620CDD69525C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -122,8 +122,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -438,18 +439,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1070FDF1-C58D-47F4-AFC4-17883B761E7D}">
-  <dimension ref="A3:D17"/>
+  <dimension ref="A3:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.73046875" customWidth="1"/>
+    <col min="1" max="1" width="20.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>0</v>
       </c>
@@ -460,7 +461,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -468,7 +469,7 @@
         <v>754130</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -476,7 +477,7 @@
         <v>746810</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -487,7 +488,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -502,7 +503,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -510,7 +511,7 @@
         <v>6247</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -518,7 +519,7 @@
         <v>6058</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -526,7 +527,7 @@
         <v>5718</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -534,7 +535,7 @@
         <v>5330</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -542,7 +543,7 @@
         <v>5251</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>15</v>
       </c>
@@ -550,7 +551,7 @@
         <v>5127</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>16</v>
       </c>
@@ -559,7 +560,7 @@
         <v>5087</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -570,10 +571,20 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="17" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B17">
         <f>B14-B15</f>
         <v>955</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="F19">
+        <f>B7-C7</f>
+        <v>15418</v>
+      </c>
+      <c r="G19" s="1">
+        <f>F19/C7</f>
+        <v>6.13517438968584E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>